<commit_message>
Update tinh lam ngoai gio, dang thieu phan goi danh sach worknote
</commit_message>
<xml_diff>
--- a/HumanResoureAPI/Resources/ExportFile/ParaFile/myfile.xlsx
+++ b/HumanResoureAPI/Resources/ExportFile/ParaFile/myfile.xlsx
@@ -1,100 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
-  <bookViews>
-    <workbookView activeTab="1" showSheetTabs="1"/>
-  </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
-    <sheet name="Evaluation Warning" sheetId="2" r:id="rId4"/>
   </sheets>
-  <calcPr fullPrecision="1" calcMode="auto" calcId="125725"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
-  <si>
-    <t>Spire.XLS for .NET</t>
-  </si>
-  <si>
-    <t>e-iceblue Inc. 2002-2020 All rights reserved</t>
-  </si>
-  <si>
-    <t>Home page</t>
-  </si>
-  <si>
-    <t>https://www.e-iceblue.com</t>
-  </si>
-  <si>
-    <t>Contact US</t>
-  </si>
-  <si>
-    <t>mailto:support@e-iceblue.com</t>
-  </si>
-  <si>
-    <t>Buy Now!</t>
-  </si>
-  <si>
-    <t>https://www.e-iceblue.com/Buy/Spire.XLS.html</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
+    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <color theme="1"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <color theme="1"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="12"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <color theme="1"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="12"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <color indexed="12"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
-      <patternFill patternType="none">
-        <bgColor indexed="65"/>
-      </patternFill>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <fgColor indexed="64"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="64"/>
-        <bgColor indexed="65"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
@@ -106,28 +39,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
-    <xf xxid="0" numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf xxid="6" numFmtId="0" fontId="3" fillId="2" borderId="0" applyAlignment="0"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs>
-    <xf xxid="1" numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" applyFill="1" applyProtection="1"/>
-    <xf xxid="2" numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf xxid="3" numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf xxid="4" numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xxid="5" numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xxid="7" numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf xxid="8" numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+  <cellXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -455,142 +374,38 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr/>
-  <dimension ref="A1:R2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView view="normal" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" baseColWidth="0"/>
   <sheetData>
-    <row r="1" spans="1:18">
-      <c r="A1" s="1">
+    <row r="1">
+      <c r="A1">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="str">
+      <c r="B1" t="str">
         <v>Theo dõi cập nhật các quy định của Pháp Luật và cập nhật QC, hướng dẫn, kiểm tra chấp hành nội quy, QC</v>
       </c>
-      <c r="C1" s="1" t="str">
+      <c r="C1" t="str">
         <v>HC401400</v>
       </c>
-      <c r="D1" s="1">
-        <v>38906.62</v>
-      </c>
-      <c r="E1" s="1">
-        <v>1.1</v>
-      </c>
-      <c r="F1" s="1">
-        <v>1</v>
-      </c>
-      <c r="G1" s="1">
-        <v>42797.28</v>
-      </c>
-      <c r="H1" s="1">
-        <v>100</v>
-      </c>
-      <c r="I1" s="1">
-        <v>1</v>
-      </c>
-      <c r="J1" s="1">
-        <v>0</v>
-      </c>
-      <c r="K1" s="1">
-        <v>0</v>
-      </c>
-      <c r="L1" s="1">
-        <v>0</v>
-      </c>
-      <c r="M1" s="1">
-        <v>0</v>
-      </c>
-      <c r="N1" s="1">
-        <v>0</v>
-      </c>
-      <c r="O1" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q1" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="R1" s="1">
-        <v>99.5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" s="1" t="str">
-        <v>Hiệu quả công việc: 99.50 %</v>
+      <c r="D1" t="str">
+        <v>18/10/2020</v>
+      </c>
+      <c r="E1" t="str">
+        <v>21:03</v>
+      </c>
+      <c r="F1" t="str">
+        <v>08:30</v>
+      </c>
+      <c r="G1">
+        <v>6447.11</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A2:H2"/>
-  </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:S2" numberStoredAsText="1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H1"/>
   </ignoredErrors>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr/>
-  <dimension ref="B1:B11"/>
-  <sheetViews>
-    <sheetView view="normal" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" baseColWidth="0"/>
-  <sheetData>
-    <row r="1" spans="2:2">
-      <c r="B1" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="2:2">
-      <c r="B2" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="2:2">
-      <c r="B4" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2">
-      <c r="B5" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="2:2">
-      <c r="B7" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="2:2">
-      <c r="B8" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="2:2">
-      <c r="B10" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="2:2">
-      <c r="B11" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1"/>
-    <hyperlink ref="B8" r:id="rId2"/>
-    <hyperlink ref="B11" r:id="rId3"/>
-  </hyperlinks>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
update bao cao sum time
</commit_message>
<xml_diff>
--- a/HumanResoureAPI/Resources/ExportFile/ParaFile/myfile.xlsx
+++ b/HumanResoureAPI/Resources/ExportFile/ParaFile/myfile.xlsx
@@ -1,33 +1,100 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <bookViews>
+    <workbookView activeTab="1" showSheetTabs="1"/>
+  </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
+    <sheet name="Evaluation Warning" sheetId="2" r:id="rId4"/>
   </sheets>
+  <calcPr fullPrecision="1" calcMode="auto" calcId="125725"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
+  <si>
+    <t>Spire.XLS for .NET</t>
+  </si>
+  <si>
+    <t>e-iceblue Inc. 2002-2020 All rights reserved</t>
+  </si>
+  <si>
+    <t>Home page</t>
+  </si>
+  <si>
+    <t>https://www.e-iceblue.com</t>
+  </si>
+  <si>
+    <t>Contact US</t>
+  </si>
+  <si>
+    <t>mailto:support@e-iceblue.com</t>
+  </si>
+  <si>
+    <t>Buy Now!</t>
+  </si>
+  <si>
+    <t>https://www.e-iceblue.com/Buy/Spire.XLS.html</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
+<styleSheet xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
+    <numFmt numFmtId="164" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="4">
     <font>
       <sz val="12"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color theme="1"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color theme="1"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color indexed="12"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill patternType="none">
+        <bgColor indexed="65"/>
+      </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="gray125">
+        <fgColor indexed="64"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="64"/>
+        <bgColor indexed="65"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -39,14 +106,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="2">
+    <xf xxid="0" numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf xxid="6" numFmtId="0" fontId="3" fillId="2" borderId="0" applyAlignment="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+  <cellXfs>
+    <xf xxid="1" numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" applyFill="1" applyProtection="1"/>
+    <xf xxid="2" numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf xxid="3" numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf xxid="4" numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xxid="5" numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xxid="7" numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf xxid="8" numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -374,38 +455,354 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H1"/>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr/>
+  <dimension ref="A1:R6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView view="normal" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" baseColWidth="0"/>
   <sheetData>
-    <row r="1">
-      <c r="A1">
+    <row r="1" spans="1:18">
+      <c r="A1" s="1">
         <v>1</v>
       </c>
-      <c r="B1" t="str">
+      <c r="B1" s="1" t="str">
+        <v>Công tác văn thư, lưu trữ</v>
+      </c>
+      <c r="C1" s="1" t="str">
+        <v>HC200500</v>
+      </c>
+      <c r="D1" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="E1" s="1">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1">
+        <v>1</v>
+      </c>
+      <c r="G1" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="H1" s="1">
+        <v>0.52</v>
+      </c>
+      <c r="I1" s="1">
+        <v>0</v>
+      </c>
+      <c r="J1" s="1">
+        <v>0</v>
+      </c>
+      <c r="K1" s="1">
+        <v>0</v>
+      </c>
+      <c r="L1" s="1">
+        <v>0</v>
+      </c>
+      <c r="M1" s="1">
+        <v>0</v>
+      </c>
+      <c r="N1" s="1">
+        <v>0</v>
+      </c>
+      <c r="O1" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q1" s="1">
+        <v>0</v>
+      </c>
+      <c r="R1" s="1">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="A2" s="1">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="str">
+        <v>Lễ tân</v>
+      </c>
+      <c r="C2" s="1" t="str">
+        <v>HC200600</v>
+      </c>
+      <c r="D2" s="1">
+        <v>6.62</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1">
+        <v>5.96</v>
+      </c>
+      <c r="H2" s="1">
+        <v>6.21</v>
+      </c>
+      <c r="I2" s="1">
+        <v>0</v>
+      </c>
+      <c r="J2" s="1">
+        <v>0</v>
+      </c>
+      <c r="K2" s="1">
+        <v>0</v>
+      </c>
+      <c r="L2" s="1">
+        <v>0</v>
+      </c>
+      <c r="M2" s="1">
+        <v>0</v>
+      </c>
+      <c r="N2" s="1">
+        <v>0</v>
+      </c>
+      <c r="O2" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>0</v>
+      </c>
+      <c r="R2" s="1">
+        <v>6.21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
+      <c r="A3" s="1">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="str">
         <v>Theo dõi cập nhật các quy định của Pháp Luật và cập nhật QC, hướng dẫn, kiểm tra chấp hành nội quy, QC</v>
       </c>
-      <c r="C1" t="str">
+      <c r="C3" s="1" t="str">
         <v>HC401400</v>
       </c>
-      <c r="D1" t="str">
-        <v>18/10/2020</v>
-      </c>
-      <c r="E1" t="str">
-        <v>21:03</v>
-      </c>
-      <c r="F1" t="str">
-        <v>08:30</v>
-      </c>
-      <c r="G1">
-        <v>6447.11</v>
+      <c r="D3" s="1">
+        <v>64.24</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1.1</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1">
+        <v>70.66</v>
+      </c>
+      <c r="H3" s="1">
+        <v>73.62</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0</v>
+      </c>
+      <c r="L3" s="1">
+        <v>0</v>
+      </c>
+      <c r="M3" s="1">
+        <v>0</v>
+      </c>
+      <c r="N3" s="1">
+        <v>0</v>
+      </c>
+      <c r="O3" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="R3" s="1">
+        <v>73.57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
+      <c r="A4" s="1">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="str">
+        <v>Công tác bảo vệ</v>
+      </c>
+      <c r="C4" s="1" t="str">
+        <v>HC502000</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0</v>
+      </c>
+      <c r="L4" s="1">
+        <v>0</v>
+      </c>
+      <c r="M4" s="1">
+        <v>0</v>
+      </c>
+      <c r="N4" s="1">
+        <v>0</v>
+      </c>
+      <c r="O4" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>0</v>
+      </c>
+      <c r="R4" s="1">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
+      <c r="A5" s="1">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1" t="str">
+        <v>Tổng hợp ngày công phục vụ việc tính lương</v>
+      </c>
+      <c r="C5" s="1" t="str">
+        <v>HC702600</v>
+      </c>
+      <c r="D5" s="1">
+        <v>15.57</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1.1</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1.1</v>
+      </c>
+      <c r="G5" s="1">
+        <v>18.84</v>
+      </c>
+      <c r="H5" s="1">
+        <v>19.63</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0</v>
+      </c>
+      <c r="K5" s="1">
+        <v>0</v>
+      </c>
+      <c r="L5" s="1">
+        <v>0</v>
+      </c>
+      <c r="M5" s="1">
+        <v>0</v>
+      </c>
+      <c r="N5" s="1">
+        <v>0</v>
+      </c>
+      <c r="O5" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>0</v>
+      </c>
+      <c r="R5" s="1">
+        <v>19.63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="1" t="str">
+        <v>Hiệu quả công việc: 99.95 %</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A6:H6"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H1"/>
+    <ignoredError sqref="A1:S6" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr/>
+  <dimension ref="B1:B11"/>
+  <sheetViews>
+    <sheetView view="normal" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" baseColWidth="0"/>
+  <sheetData>
+    <row r="1" spans="2:2">
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="2:2">
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2">
+      <c r="B4" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2">
+      <c r="B5" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2">
+      <c r="B7" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2">
+      <c r="B8" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2">
+      <c r="B10" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2">
+      <c r="B11" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B5" r:id="rId1"/>
+    <hyperlink ref="B8" r:id="rId2"/>
+    <hyperlink ref="B11" r:id="rId3"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>